<commit_message>
Login and ManagerEmployee functionality
</commit_message>
<xml_diff>
--- a/src/main/resources/LoginData.xlsx
+++ b/src/main/resources/LoginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sweetasingh\SkillUp-Web-Automation\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E543820-A45F-4376-9F6F-9C0AD4472782}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1079C898-098B-411E-AECB-C51DC0811F76}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>UserNames</t>
   </si>
@@ -43,24 +43,6 @@
   </si>
   <si>
     <t>abc1234</t>
-  </si>
-  <si>
-    <t>adminMentor</t>
-  </si>
-  <si>
-    <t>ABC123</t>
-  </si>
-  <si>
-    <t>sangeeta</t>
-  </si>
-  <si>
-    <t>sangeeta123</t>
-  </si>
-  <si>
-    <t>sweetapal</t>
-  </si>
-  <si>
-    <t>sweeta123</t>
   </si>
   <si>
     <t>Valid</t>
@@ -407,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -439,7 +421,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -450,58 +432,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Login and Project Manager Employee functionality
</commit_message>
<xml_diff>
--- a/src/main/resources/LoginData.xlsx
+++ b/src/main/resources/LoginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sweetasingh\SkillUp-Web-Automation\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1079C898-098B-411E-AECB-C51DC0811F76}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8FB8647-8F2D-4859-95FF-895A8F515EE0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>UserNames</t>
   </si>
@@ -49,6 +49,27 @@
   </si>
   <si>
     <t>Invalid</t>
+  </si>
+  <si>
+    <t>adminMentor</t>
+  </si>
+  <si>
+    <t>studentAdmin</t>
+  </si>
+  <si>
+    <t>xyz123</t>
+  </si>
+  <si>
+    <t>sangeeta</t>
+  </si>
+  <si>
+    <t>sangeeta123</t>
+  </si>
+  <si>
+    <t>sweetapal</t>
+  </si>
+  <si>
+    <t>sweeta123</t>
   </si>
 </sst>
 </file>
@@ -389,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -435,6 +456,50 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>